<commit_message>
Update PDF and BOM
</commit_message>
<xml_diff>
--- a/Power_Board_2/BOM/Bill of Materials-Power_Board_2.xlsx
+++ b/Power_Board_2/BOM/Bill of Materials-Power_Board_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvicca0_onmicrosoft_com/Documents/University/Clubs/AUVic/Hardware/PCB-Power_Board_2/Power_Board_2/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE4F3ABF-5A45-43A6-B9F9-154F994F223A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F84853-B0AD-4AB6-A2A9-25447FA16F10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{1B9E0BC4-0F48-4359-BBA8-4FA42D101EEB}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{4D4091D8-52CC-4943-815F-AB9F39EBE83E}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Power_Board_2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Line #</t>
   </si>
@@ -70,6 +70,108 @@
   </si>
   <si>
     <t>Supplier Subtotal 1</t>
+  </si>
+  <si>
+    <t>0.015uF</t>
+  </si>
+  <si>
+    <t>Capacitor, Ceramic, 50V, +/-10%, 0603 SMD, X7R</t>
+  </si>
+  <si>
+    <t>C?</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1uF 25V 0603 SMD, Ceramic</t>
+  </si>
+  <si>
+    <t>Capacitor, Ceramic, 25V, +/- 10%, 0603 SMD, X5R</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>Capacitor, Ceramic, 50V, +/- 10%, 1206 SMD, X7R</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>Capacitor, Ceramic, 10V, +/- 10%, 0805 SMD, X5R</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V 10% X7R 1608 (0603)</t>
+  </si>
+  <si>
+    <t>CMP-057-0013-1</t>
+  </si>
+  <si>
+    <t>Diode, Schottky, 60V, 2A</t>
+  </si>
+  <si>
+    <t>D?</t>
+  </si>
+  <si>
+    <t>LED, 0805 (2012), Green, Clear</t>
+  </si>
+  <si>
+    <t>6.8µH</t>
+  </si>
+  <si>
+    <t>6.8uH 1.06A</t>
+  </si>
+  <si>
+    <t>L?</t>
+  </si>
+  <si>
+    <t>3.9k</t>
+  </si>
+  <si>
+    <t>3.9k, 5%, 1/8W, 0805 SMD</t>
+  </si>
+  <si>
+    <t>R?</t>
+  </si>
+  <si>
+    <t>100R, 1%, 1/10W, 0603 SMD</t>
+  </si>
+  <si>
+    <t>150R, 1%, 1/10W, 0603, SMD</t>
+  </si>
+  <si>
+    <t>RES SMD 150 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>680</t>
+  </si>
+  <si>
+    <t>680, 5%, 1/8W, 0805 SMD</t>
+  </si>
+  <si>
+    <t>3.3V 250mA Linear Reg LDO</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 250MA SOT23-3</t>
+  </si>
+  <si>
+    <t>U?</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>AP2138N-3.3TRG1</t>
+  </si>
+  <si>
+    <t>CMP-045-0010-1</t>
+  </si>
+  <si>
+    <t>DC-DC Regulator, 6V-42V in, 1V-29.4V out, 500mA</t>
   </si>
 </sst>
 </file>
@@ -126,10 +228,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -445,11 +553,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B73FDEB-9CC3-49FD-89F8-71F8A8527C0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6DBED1-9491-41BC-842E-990728170FCA}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -506,10 +614,328 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -772,7 +1198,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD108D96-26B6-4DF9-866D-F67E915D51AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E34E76-02A0-4044-9771-542F84ED0FF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -792,7 +1218,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4607CD3-1B74-45C5-86B0-ED8F5677CDA6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD44A3E-E686-4820-AEB7-019F4ECB0F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -800,19 +1226,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4398BF-13E3-4FB8-B6B0-EA0E5BCA0D03}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43A3334-3D4D-4AA5-9149-30D94EBC5DE8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="8966a34b-ec6c-46f3-826c-d8f2f7d74935"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="5c534bb1-62b0-46e0-9ae3-b9112d146ccd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finalized LEDs and LED resistors
</commit_message>
<xml_diff>
--- a/Power_Board_2/BOM/Bill of Materials-Power_Board_2.xlsx
+++ b/Power_Board_2/BOM/Bill of Materials-Power_Board_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvicca0_onmicrosoft_com/Documents/University/Clubs/AUVic/Hardware/PCB-Power_Board_2/Power_Board_2/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{687411CE-57AF-473F-BA63-A62D128370D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{687411CE-57AF-473F-BA63-A62D128370D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7B2042F-526C-47AB-979B-FF0E17339F69}"/>
   <bookViews>
-    <workbookView xWindow="-25965" yWindow="1155" windowWidth="17280" windowHeight="9420" xr2:uid="{661FFB2B-6F0B-49C8-B54D-7B2428E1D6C5}"/>
+    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="13824" windowHeight="7536" xr2:uid="{661FFB2B-6F0B-49C8-B54D-7B2428E1D6C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Power_Board_2" sheetId="1" r:id="rId1"/>
@@ -1870,9 +1870,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C102" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5579,6 +5581,18 @@
         <v>1.49</v>
       </c>
     </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E103">
+        <f>SUM(E2:E102)</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E1048576">
+        <f>SUM(E2:E1048575)</f>
+        <v>624</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
@@ -5587,6 +5601,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024846BE2D35DE54A9BE8BBA42D0700AD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="641b7ec275f27219802da9e743dd1056">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="5c534bb1-62b0-46e0-9ae3-b9112d146ccd" xmlns:ns4="8966a34b-ec6c-46f3-826c-d8f2f7d74935" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1271ae291c08be0062a66eeb80c51a0" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5826,25 +5858,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59FB213-C6F3-4341-90CA-6EDA6233E525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1734F637-A3F2-4D44-B203-EAC367008C26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3E756C-6DCA-494A-BCBE-B5B7FF9F9C66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5862,22 +5894,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1734F637-A3F2-4D44-B203-EAC367008C26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59FB213-C6F3-4341-90CA-6EDA6233E525}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>